<commit_message>
One texture per model
</commit_message>
<xml_diff>
--- a/6044_FramPat/SAM/Project #1/Robotron 2084/Sprite map/sprite - Daddy.xlsx
+++ b/6044_FramPat/SAM/Project #1/Robotron 2084/Sprite map/sprite - Daddy.xlsx
@@ -281,7 +281,7 @@
         <xdr:cNvPr id="1030" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -327,7 +327,7 @@
         <xdr:cNvPr id="1032" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -373,7 +373,7 @@
         <xdr:cNvPr id="1034" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -419,7 +419,7 @@
         <xdr:cNvPr id="1036" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -465,7 +465,7 @@
         <xdr:cNvPr id="1038" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -511,7 +511,7 @@
         <xdr:cNvPr id="1040" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -557,7 +557,7 @@
         <xdr:cNvPr id="1042" name="Picture 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000012040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -603,7 +603,7 @@
         <xdr:cNvPr id="1044" name="Picture 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000014040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -649,7 +649,7 @@
         <xdr:cNvPr id="1046" name="Picture 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -695,7 +695,7 @@
         <xdr:cNvPr id="1048" name="Picture 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -741,7 +741,7 @@
         <xdr:cNvPr id="1050" name="Picture 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001A040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -787,7 +787,7 @@
         <xdr:cNvPr id="1052" name="Picture 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001C040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -806,6 +806,201 @@
         <a:xfrm>
           <a:off x="13446672" y="6260224"/>
           <a:ext cx="1522649" cy="2489639"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>80</xdr:col>
+      <xdr:colOff>116054</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>177376</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>87</xdr:col>
+      <xdr:colOff>152978</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>142804</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15746823" y="9829376"/>
+          <a:ext cx="1404617" cy="2378428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>81765</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>151424</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>115151</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>106358</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12000227" y="9432193"/>
+          <a:ext cx="3159539" cy="3110396"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>43962</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>4036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>52033</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>54581</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="TextBox 15"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8836270" y="12811498"/>
+          <a:ext cx="8409609" cy="607391"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>At the beginning of this: https://www.youtube.com/watch?v=l800GL6NQPY&amp;t=435s&amp;ab_channel=OldClassicRetroGaming the progs seem</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> to be one of the "poses" of the model where the colours flash. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>175846</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>34191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>158261</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>161191</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="957384" y="9314960"/>
+          <a:ext cx="7407031" cy="5695462"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1105,13 +1300,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="BJ34" sqref="BJ34:BR46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AC59" sqref="AC59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="96" width="2.85546875" customWidth="1"/>
+    <col min="1" max="96" width="2.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73">
@@ -6349,7 +6544,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6361,7 +6556,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>